<commit_message>
update department codes in excel
</commit_message>
<xml_diff>
--- a/uploads/format/Purchase Request.xlsx
+++ b/uploads/format/Purchase Request.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F64A458-714F-4B09-B884-6212C392E530}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5100"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Department Code" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -87,12 +89,141 @@
   </si>
   <si>
     <t>(Y-m-d)</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>HR - BCD</t>
+  </si>
+  <si>
+    <t>HRB</t>
+  </si>
+  <si>
+    <t>Billing Department</t>
+  </si>
+  <si>
+    <t>BIL</t>
+  </si>
+  <si>
+    <t>EIC</t>
+  </si>
+  <si>
+    <t>Environment/PCO</t>
+  </si>
+  <si>
+    <t>ENV</t>
+  </si>
+  <si>
+    <t>Finance Department</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>Fuel and Lube Management</t>
+  </si>
+  <si>
+    <t>FLM</t>
+  </si>
+  <si>
+    <t>Health and Safety</t>
+  </si>
+  <si>
+    <t>HAS</t>
+  </si>
+  <si>
+    <t>IT Department - BCD</t>
+  </si>
+  <si>
+    <t>ITB</t>
+  </si>
+  <si>
+    <t>IT Department - SITE</t>
+  </si>
+  <si>
+    <t>ITS</t>
+  </si>
+  <si>
+    <t>Laboratory and Chemical</t>
+  </si>
+  <si>
+    <t>LAB</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>MAI</t>
+  </si>
+  <si>
+    <t>Office of the GM</t>
+  </si>
+  <si>
+    <t>OOG</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>OPE</t>
+  </si>
+  <si>
+    <t>Purchasing Department</t>
+  </si>
+  <si>
+    <t>PUR</t>
+  </si>
+  <si>
+    <t>Reconditioning</t>
+  </si>
+  <si>
+    <t>REC</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>SEC</t>
+  </si>
+  <si>
+    <t>HR - SITE</t>
+  </si>
+  <si>
+    <t>HRS</t>
+  </si>
+  <si>
+    <t>Special Proj/Facilities Imp</t>
+  </si>
+  <si>
+    <t>SPE</t>
+  </si>
+  <si>
+    <t>Trading Department</t>
+  </si>
+  <si>
+    <t>TRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warehouse - CENPRI </t>
+  </si>
+  <si>
+    <t>WHC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warehouse - Progen </t>
+  </si>
+  <si>
+    <t>WHP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -405,7 +536,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -699,11 +836,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:K24"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,4 +1183,198 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632B8BD7-0760-4950-A21C-269F6E5E404C}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new db and pr format
</commit_message>
<xml_diff>
--- a/uploads/format/Purchase Request.xlsx
+++ b/uploads/format/Purchase Request.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F64A458-714F-4B09-B884-6212C392E530}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554BCBAB-CE85-485D-AB99-8FE6CA3371A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>WHP</t>
+  </si>
+  <si>
+    <t>Dept. Code</t>
+  </si>
+  <si>
+    <t>(refer to department code sheet)</t>
   </si>
 </sst>
 </file>
@@ -227,7 +233,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +260,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -408,7 +422,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -416,7 +429,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -424,66 +436,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -493,7 +445,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -840,7 +858,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,294 +882,312 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="20" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="11"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="22" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="12"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="23" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="12"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="16" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="19"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="34"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="27"/>
       <c r="H7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="26"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="29"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="24" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="H8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="18"/>
+      <c r="H8" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="26"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="26" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="27"/>
+      <c r="D9" s="26"/>
       <c r="E9" s="27"/>
       <c r="H9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="25"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
+      <c r="H10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="29"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="8"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="27"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="29"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="32"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="33" t="s">
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="34"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="24" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="39"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="24" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="39"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="24" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="39"/>
+      <c r="K16" s="18"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="24" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="39"/>
+      <c r="K17" s="18"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="24" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="K18" s="39"/>
+      <c r="K18" s="18"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="24" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="K19" s="39"/>
+      <c r="K19" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
+  <mergeCells count="33">
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C7:E7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:I13"/>
     <mergeCell ref="E14:I14"/>
@@ -1160,24 +1196,12 @@
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="J16:K16"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>